<commit_message>
cambios en diseño de daysi
cambios en diseño de daysi
</commit_message>
<xml_diff>
--- a/padronn-web/src/main/webapp/WEB-INF/formato/Actas_Municipios_Cumplieron.xlsx
+++ b/padronn-web/src/main/webapp/WEB-INF/formato/Actas_Municipios_Cumplieron.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="23580" windowHeight="9855"/>
@@ -217,31 +217,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,8 +551,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
@@ -565,60 +565,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="11" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="16"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="7" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>